<commit_message>
adicionado documento de endpoints
</commit_message>
<xml_diff>
--- a/Documentacao/Requisitos.xlsx
+++ b/Documentacao/Requisitos.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositorios\ISEL\PS\ProjectoFInal\Documentacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AA6F2D37-1ED7-42C1-9471-562167A50F47}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B871B82C-1894-4AAE-B5EB-016B8CFB7AB1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="13176" xr2:uid="{EAAEDE45-132D-4245-87D6-128065722018}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
-    <sheet name="Folha2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="59">
   <si>
     <t>Requisito</t>
   </si>
@@ -211,6 +210,9 @@
   <si>
     <t>utilizador tem de estar logado para submeter questoes.
 Apenas utilizadores logados podem consultar historica</t>
+  </si>
+  <si>
+    <t>X</t>
   </si>
 </sst>
 </file>
@@ -234,15 +236,33 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEB6553"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -250,11 +270,235 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -268,13 +512,112 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -283,6 +626,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFEB6553"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -591,10 +939,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23C641B3-BD7E-4177-911B-D187B756B533}">
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -604,294 +952,393 @@
     <col min="3" max="3" width="29.21875" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.88671875" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="32.109375" style="3" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="2"/>
+    <col min="6" max="6" width="13.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" customFormat="1" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" customFormat="1" ht="51.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="5" t="s">
+    <row r="2" spans="1:8" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="G2" t="s">
+      <c r="F2" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="H2" t="s">
+      <c r="G2" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="I2" t="s">
+      <c r="H2" s="28" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B3" s="2" t="s">
+    <row r="3" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B3" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B4" s="2" t="s">
+      <c r="E3" s="35"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="14" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B4" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="7" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B5" s="2" t="s">
+      <c r="E4" s="36"/>
+      <c r="F4" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="G4" s="7"/>
+      <c r="H4" s="16"/>
+    </row>
+    <row r="5" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B5" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="7" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B6" s="2" t="s">
+      <c r="E5" s="36"/>
+      <c r="F5" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="G5" s="7"/>
+      <c r="H5" s="16"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B6" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="9" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="B7" s="2" t="s">
+      <c r="E6" s="37"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="H6" s="18"/>
+    </row>
+    <row r="7" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="B7" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="36" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B8" s="2" t="s">
+      <c r="F7" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="G7" s="7"/>
+      <c r="H7" s="16"/>
+    </row>
+    <row r="8" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B8" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="36" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" ht="72" x14ac:dyDescent="0.3">
-      <c r="B9" s="2" t="s">
+      <c r="F8" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="G8" s="7"/>
+      <c r="H8" s="16"/>
+    </row>
+    <row r="9" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+      <c r="B9" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="36" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B10" s="2" t="s">
+      <c r="F9" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="G9" s="7"/>
+      <c r="H9" s="16"/>
+    </row>
+    <row r="10" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B10" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="7" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B11" s="2" t="s">
+      <c r="E10" s="36"/>
+      <c r="F10" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="G10" s="7"/>
+      <c r="H10" s="16"/>
+    </row>
+    <row r="11" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B11" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="9" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B12" s="2" t="s">
+      <c r="E11" s="37"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="H11" s="18"/>
+    </row>
+    <row r="12" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B12" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E12" s="36" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B13" s="2" t="s">
+      <c r="F12" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="G12" s="7"/>
+      <c r="H12" s="16"/>
+    </row>
+    <row r="13" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B13" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="7" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B14" s="2" t="s">
+      <c r="E13" s="36"/>
+      <c r="F13" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="G13" s="7"/>
+      <c r="H13" s="16"/>
+    </row>
+    <row r="14" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B14" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="D14" s="9"/>
+      <c r="E14" s="37" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B15" s="2" t="s">
+      <c r="F14" s="32"/>
+      <c r="G14" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="H14" s="18"/>
+    </row>
+    <row r="15" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B15" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="E15" s="7"/>
-    </row>
-    <row r="16" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B16" s="2" t="s">
+      <c r="E15" s="38"/>
+      <c r="F15" s="33"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="20" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B16" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D16" s="5" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="17" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B17" s="2" t="s">
+      <c r="E16" s="39"/>
+      <c r="F16" s="33"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="20" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B17" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D17" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="E17" s="37" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="18" spans="2:5" ht="72" x14ac:dyDescent="0.3">
-      <c r="B18" s="2" t="s">
+      <c r="F17" s="32"/>
+      <c r="G17" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="H17" s="18"/>
+    </row>
+    <row r="18" spans="2:8" ht="72" x14ac:dyDescent="0.3">
+      <c r="B18" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D18" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="E18" s="37" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="19" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B19" s="2" t="s">
+      <c r="F18" s="32"/>
+      <c r="G18" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="H18" s="18"/>
+    </row>
+    <row r="19" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B19" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D19" s="9" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="20" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B20" s="2" t="s">
+      <c r="E19" s="37"/>
+      <c r="F19" s="32"/>
+      <c r="G19" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="H19" s="18"/>
+    </row>
+    <row r="20" spans="2:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B20" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D20" s="7" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="21" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B21" s="2" t="s">
+      <c r="E20" s="36"/>
+      <c r="F20" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="G20" s="7"/>
+      <c r="H20" s="16"/>
+    </row>
+    <row r="21" spans="2:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B21" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C21" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D21" s="5" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="22" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B22" s="2" t="s">
+      <c r="E21" s="39"/>
+      <c r="F21" s="33"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="20" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C22" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D22" s="23" t="s">
         <v>42</v>
+      </c>
+      <c r="E22" s="40"/>
+      <c r="F22" s="34"/>
+      <c r="G22" s="23"/>
+      <c r="H22" s="24" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{653E6311-A337-499A-BDC5-9FD06898DC20}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>